<commit_message>
SMB warpless - 3-2 done
</commit_message>
<xml_diff>
--- a/trunk/SMB/SMB.xlsx
+++ b/trunk/SMB/SMB.xlsx
@@ -1962,6 +1962,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2079,9 +2082,6 @@
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2393,7 +2393,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -2410,16 +2410,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="161" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65520)</f>
@@ -2497,10 +2497,10 @@
       <c r="B5" s="145" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>206</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="145"/>
       <c r="F5" s="141"/>
       <c r="G5" s="138"/>
@@ -2516,12 +2516,12 @@
       <c r="B6" s="145" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="159"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
       <c r="G6" s="138"/>
       <c r="H6" s="138"/>
       <c r="I6" s="138"/>
@@ -2537,7 +2537,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>204</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2557,7 +2557,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A9" s="155"/>
+      <c r="A9" s="156"/>
       <c r="B9" s="98" t="s">
         <v>175</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A10" s="155"/>
+      <c r="A10" s="156"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2578,7 +2578,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A11" s="155"/>
+      <c r="A11" s="156"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2589,7 +2589,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A12" s="155"/>
+      <c r="A12" s="156"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2600,7 +2600,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A13" s="155"/>
+      <c r="A13" s="156"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2611,7 +2611,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A14" s="155"/>
+      <c r="A14" s="156"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2622,7 +2622,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A15" s="155"/>
+      <c r="A15" s="156"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2633,7 +2633,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A16" s="155"/>
+      <c r="A16" s="156"/>
       <c r="B16" s="98" t="s">
         <v>177</v>
       </c>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="157" t="s">
         <v>209</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2696,7 +2696,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="155"/>
+      <c r="A20" s="156"/>
       <c r="B20" s="98" t="s">
         <v>175</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A21" s="155"/>
+      <c r="A21" s="156"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2720,7 +2720,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A22" s="155"/>
+      <c r="A22" s="156"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2731,7 +2731,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A23" s="155"/>
+      <c r="A23" s="156"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2742,7 +2742,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A24" s="155"/>
+      <c r="A24" s="156"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2753,7 +2753,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A25" s="155"/>
+      <c r="A25" s="156"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2764,7 +2764,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A26" s="155"/>
+      <c r="A26" s="156"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2775,7 +2775,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A27" s="155"/>
+      <c r="A27" s="156"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2786,7 +2786,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A28" s="155"/>
+      <c r="A28" s="156"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2797,7 +2797,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A29" s="155"/>
+      <c r="A29" s="156"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2808,7 +2808,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A30" s="155"/>
+      <c r="A30" s="156"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2819,7 +2819,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A31" s="155"/>
+      <c r="A31" s="156"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2830,7 +2830,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A32" s="155"/>
+      <c r="A32" s="156"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2841,7 +2841,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A33" s="155"/>
+      <c r="A33" s="156"/>
       <c r="B33" s="98" t="s">
         <v>177</v>
       </c>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A36" s="154" t="s">
+      <c r="A36" s="155" t="s">
         <v>208</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2900,7 +2900,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A37" s="155"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="98" t="s">
         <v>175</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A38" s="155"/>
+      <c r="A38" s="156"/>
       <c r="B38" s="153" t="s">
         <v>222</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A39" s="155"/>
+      <c r="A39" s="156"/>
       <c r="B39" s="153" t="s">
         <v>223</v>
       </c>
@@ -2951,8 +2951,8 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A40" s="155"/>
-      <c r="B40" s="219" t="s">
+      <c r="A40" s="156"/>
+      <c r="B40" s="154" t="s">
         <v>224</v>
       </c>
       <c r="C40" s="101"/>
@@ -2966,8 +2966,8 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A41" s="155"/>
-      <c r="B41" s="219" t="s">
+      <c r="A41" s="156"/>
+      <c r="B41" s="154" t="s">
         <v>226</v>
       </c>
       <c r="C41" s="101">
@@ -2983,22 +2983,24 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A42" s="155"/>
-      <c r="B42" s="219" t="s">
+      <c r="A42" s="156"/>
+      <c r="B42" s="154" t="s">
         <v>225</v>
       </c>
-      <c r="C42" s="101"/>
+      <c r="C42" s="101">
+        <v>21459</v>
+      </c>
       <c r="D42" s="101">
         <v>21564</v>
       </c>
       <c r="E42" s="121">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A43" s="155"/>
+      <c r="A43" s="156"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3009,7 +3011,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A44" s="155"/>
+      <c r="A44" s="156"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3020,7 +3022,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A45" s="155"/>
+      <c r="A45" s="156"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3031,7 +3033,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A46" s="155"/>
+      <c r="A46" s="156"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3042,7 +3044,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A47" s="155"/>
+      <c r="A47" s="156"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3053,7 +3055,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A48" s="155"/>
+      <c r="A48" s="156"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3064,7 +3066,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="155"/>
+      <c r="A49" s="156"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3075,7 +3077,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A50" s="155"/>
+      <c r="A50" s="156"/>
       <c r="B50" s="100"/>
       <c r="C50" s="101"/>
       <c r="D50" s="101"/>
@@ -3086,7 +3088,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A51" s="155"/>
+      <c r="A51" s="156"/>
       <c r="B51" s="98" t="s">
         <v>177</v>
       </c>
@@ -3125,7 +3127,7 @@
     </row>
     <row r="53" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="54" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A54" s="156" t="s">
+      <c r="A54" s="157" t="s">
         <v>212</v>
       </c>
       <c r="B54" s="109" t="s">
@@ -3145,7 +3147,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A55" s="155"/>
+      <c r="A55" s="156"/>
       <c r="B55" s="98" t="s">
         <v>175</v>
       </c>
@@ -3158,7 +3160,7 @@
       <c r="F55" s="104"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A56" s="155"/>
+      <c r="A56" s="156"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3169,7 +3171,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A57" s="155"/>
+      <c r="A57" s="156"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3180,7 +3182,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A58" s="155"/>
+      <c r="A58" s="156"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3191,7 +3193,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A59" s="155"/>
+      <c r="A59" s="156"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3202,7 +3204,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A60" s="155"/>
+      <c r="A60" s="156"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3213,7 +3215,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A61" s="155"/>
+      <c r="A61" s="156"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3224,7 +3226,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A62" s="155"/>
+      <c r="A62" s="156"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3235,7 +3237,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A63" s="155"/>
+      <c r="A63" s="156"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3246,7 +3248,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A64" s="155"/>
+      <c r="A64" s="156"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3257,7 +3259,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A65" s="155"/>
+      <c r="A65" s="156"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3268,7 +3270,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A66" s="155"/>
+      <c r="A66" s="156"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3279,7 +3281,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A67" s="155"/>
+      <c r="A67" s="156"/>
       <c r="B67" s="100"/>
       <c r="C67" s="101"/>
       <c r="D67" s="101"/>
@@ -3290,7 +3292,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A68" s="155"/>
+      <c r="A68" s="156"/>
       <c r="B68" s="98" t="s">
         <v>177</v>
       </c>
@@ -3329,7 +3331,7 @@
     </row>
     <row r="70" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="71" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A71" s="154" t="s">
+      <c r="A71" s="155" t="s">
         <v>215</v>
       </c>
       <c r="B71" s="113" t="s">
@@ -3349,7 +3351,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A72" s="155"/>
+      <c r="A72" s="156"/>
       <c r="B72" s="98" t="s">
         <v>175</v>
       </c>
@@ -3362,7 +3364,7 @@
       <c r="F72" s="104"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A73" s="155"/>
+      <c r="A73" s="156"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3373,7 +3375,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A74" s="155"/>
+      <c r="A74" s="156"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3384,7 +3386,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A75" s="155"/>
+      <c r="A75" s="156"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3395,7 +3397,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A76" s="155"/>
+      <c r="A76" s="156"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3406,7 +3408,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A77" s="155"/>
+      <c r="A77" s="156"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3417,7 +3419,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A78" s="155"/>
+      <c r="A78" s="156"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3428,7 +3430,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A79" s="155"/>
+      <c r="A79" s="156"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3439,7 +3441,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A80" s="155"/>
+      <c r="A80" s="156"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3450,7 +3452,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A81" s="155"/>
+      <c r="A81" s="156"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3461,7 +3463,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A82" s="155"/>
+      <c r="A82" s="156"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3472,7 +3474,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A83" s="155"/>
+      <c r="A83" s="156"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3483,7 +3485,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A84" s="155"/>
+      <c r="A84" s="156"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3494,7 +3496,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A85" s="155"/>
+      <c r="A85" s="156"/>
       <c r="B85" s="98" t="s">
         <v>177</v>
       </c>
@@ -3533,7 +3535,7 @@
     </row>
     <row r="87" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="88" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A88" s="156" t="s">
+      <c r="A88" s="157" t="s">
         <v>214</v>
       </c>
       <c r="B88" s="109" t="s">
@@ -3553,7 +3555,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A89" s="155"/>
+      <c r="A89" s="156"/>
       <c r="B89" s="98" t="s">
         <v>175</v>
       </c>
@@ -3566,7 +3568,7 @@
       <c r="F89" s="104"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A90" s="155"/>
+      <c r="A90" s="156"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3577,7 +3579,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A91" s="155"/>
+      <c r="A91" s="156"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3588,7 +3590,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A92" s="155"/>
+      <c r="A92" s="156"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3599,7 +3601,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A93" s="155"/>
+      <c r="A93" s="156"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3610,7 +3612,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A94" s="155"/>
+      <c r="A94" s="156"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3621,7 +3623,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A95" s="155"/>
+      <c r="A95" s="156"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3632,7 +3634,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A96" s="155"/>
+      <c r="A96" s="156"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3643,7 +3645,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A97" s="155"/>
+      <c r="A97" s="156"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3654,7 +3656,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A98" s="155"/>
+      <c r="A98" s="156"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3665,7 +3667,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A99" s="155"/>
+      <c r="A99" s="156"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3676,7 +3678,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A100" s="155"/>
+      <c r="A100" s="156"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3687,7 +3689,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A101" s="155"/>
+      <c r="A101" s="156"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3698,7 +3700,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A102" s="155"/>
+      <c r="A102" s="156"/>
       <c r="B102" s="98" t="s">
         <v>177</v>
       </c>
@@ -3737,7 +3739,7 @@
     </row>
     <row r="104" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="105" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A105" s="154" t="s">
+      <c r="A105" s="155" t="s">
         <v>218</v>
       </c>
       <c r="B105" s="113" t="s">
@@ -3757,7 +3759,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A106" s="155"/>
+      <c r="A106" s="156"/>
       <c r="B106" s="98" t="s">
         <v>175</v>
       </c>
@@ -3770,7 +3772,7 @@
       <c r="F106" s="104"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A107" s="155"/>
+      <c r="A107" s="156"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3781,7 +3783,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A108" s="155"/>
+      <c r="A108" s="156"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3792,7 +3794,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A109" s="155"/>
+      <c r="A109" s="156"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3803,7 +3805,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A110" s="155"/>
+      <c r="A110" s="156"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3814,7 +3816,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A111" s="155"/>
+      <c r="A111" s="156"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3825,7 +3827,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A112" s="155"/>
+      <c r="A112" s="156"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3836,7 +3838,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A113" s="155"/>
+      <c r="A113" s="156"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3847,7 +3849,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A114" s="155"/>
+      <c r="A114" s="156"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3858,7 +3860,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A115" s="155"/>
+      <c r="A115" s="156"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3869,7 +3871,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A116" s="155"/>
+      <c r="A116" s="156"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3880,7 +3882,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A117" s="155"/>
+      <c r="A117" s="156"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -3891,7 +3893,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A118" s="155"/>
+      <c r="A118" s="156"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -3902,7 +3904,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A119" s="155"/>
+      <c r="A119" s="156"/>
       <c r="B119" s="98" t="s">
         <v>177</v>
       </c>
@@ -3941,7 +3943,7 @@
     </row>
     <row r="121" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="122" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A122" s="156" t="s">
+      <c r="A122" s="157" t="s">
         <v>220</v>
       </c>
       <c r="B122" s="109" t="s">
@@ -3961,7 +3963,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A123" s="155"/>
+      <c r="A123" s="156"/>
       <c r="B123" s="98" t="s">
         <v>175</v>
       </c>
@@ -3974,7 +3976,7 @@
       <c r="F123" s="104"/>
     </row>
     <row r="124" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A124" s="155"/>
+      <c r="A124" s="156"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -3985,7 +3987,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A125" s="155"/>
+      <c r="A125" s="156"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -3996,7 +3998,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A126" s="155"/>
+      <c r="A126" s="156"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4007,7 +4009,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A127" s="155"/>
+      <c r="A127" s="156"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4018,7 +4020,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A128" s="155"/>
+      <c r="A128" s="156"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4029,7 +4031,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A129" s="155"/>
+      <c r="A129" s="156"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4040,7 +4042,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A130" s="155"/>
+      <c r="A130" s="156"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4051,7 +4053,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A131" s="155"/>
+      <c r="A131" s="156"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4062,7 +4064,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A132" s="155"/>
+      <c r="A132" s="156"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4073,7 +4075,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A133" s="155"/>
+      <c r="A133" s="156"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4084,7 +4086,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A134" s="155"/>
+      <c r="A134" s="156"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4095,7 +4097,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A135" s="155"/>
+      <c r="A135" s="156"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4106,7 +4108,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A136" s="155"/>
+      <c r="A136" s="156"/>
       <c r="B136" s="98" t="s">
         <v>177</v>
       </c>
@@ -4188,13 +4190,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="183" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4224,18 +4226,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4387,9 +4389,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4540,9 +4542,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="165"/>
+      <c r="D38" s="166"/>
+      <c r="E38" s="166"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -4693,9 +4695,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="165"/>
+      <c r="D55" s="166"/>
+      <c r="E55" s="166"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -4846,9 +4848,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="165"/>
+      <c r="D72" s="166"/>
+      <c r="E72" s="166"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -4999,9 +5001,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="165"/>
+      <c r="D89" s="166"/>
+      <c r="E89" s="166"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5152,9 +5154,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="165"/>
+      <c r="D106" s="166"/>
+      <c r="E106" s="166"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5305,9 +5307,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="165"/>
+      <c r="D123" s="166"/>
+      <c r="E123" s="166"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5458,9 +5460,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="165"/>
+      <c r="D140" s="166"/>
+      <c r="E140" s="166"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5611,9 +5613,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="165"/>
+      <c r="D157" s="166"/>
+      <c r="E157" s="166"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -5764,9 +5766,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="165"/>
+      <c r="D174" s="166"/>
+      <c r="E174" s="166"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -5917,9 +5919,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="165"/>
+      <c r="D191" s="166"/>
+      <c r="E191" s="166"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6070,9 +6072,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="165"/>
+      <c r="D208" s="166"/>
+      <c r="E208" s="166"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6223,9 +6225,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="165"/>
+      <c r="D225" s="166"/>
+      <c r="E225" s="166"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6376,9 +6378,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="165"/>
+      <c r="D242" s="166"/>
+      <c r="E242" s="166"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6529,9 +6531,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="165"/>
+      <c r="D259" s="166"/>
+      <c r="E259" s="166"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -6682,18 +6684,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="181"/>
+      <c r="D276" s="182"/>
+      <c r="E276" s="182"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="165"/>
+      <c r="D277" s="166"/>
+      <c r="E277" s="166"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -6844,9 +6846,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="167"/>
+      <c r="D294" s="168"/>
+      <c r="E294" s="168"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -6997,9 +6999,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="165"/>
+      <c r="D311" s="166"/>
+      <c r="E311" s="166"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7150,9 +7152,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="165"/>
+      <c r="D328" s="166"/>
+      <c r="E328" s="166"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7303,9 +7305,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="165"/>
+      <c r="D345" s="166"/>
+      <c r="E345" s="166"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7456,9 +7458,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="165"/>
+      <c r="D362" s="166"/>
+      <c r="E362" s="166"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7609,9 +7611,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="165"/>
+      <c r="D379" s="166"/>
+      <c r="E379" s="166"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -7762,9 +7764,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="165"/>
+      <c r="D396" s="166"/>
+      <c r="E396" s="166"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -7915,9 +7917,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="165"/>
+      <c r="D413" s="166"/>
+      <c r="E413" s="166"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8068,9 +8070,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="165"/>
+      <c r="D430" s="166"/>
+      <c r="E430" s="166"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8221,9 +8223,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="165"/>
+      <c r="D447" s="166"/>
+      <c r="E447" s="166"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8374,9 +8376,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="165"/>
+      <c r="D464" s="166"/>
+      <c r="E464" s="166"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8527,9 +8529,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="165"/>
+      <c r="D481" s="166"/>
+      <c r="E481" s="166"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -8680,9 +8682,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="165"/>
+      <c r="D498" s="166"/>
+      <c r="E498" s="166"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -8833,9 +8835,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="165"/>
+      <c r="D515" s="166"/>
+      <c r="E515" s="166"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -8986,9 +8988,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="165"/>
+      <c r="D532" s="166"/>
+      <c r="E532" s="166"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9139,18 +9141,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="178"/>
-      <c r="D549" s="179"/>
-      <c r="E549" s="179"/>
+      <c r="C549" s="179"/>
+      <c r="D549" s="180"/>
+      <c r="E549" s="180"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="165"/>
+      <c r="D550" s="166"/>
+      <c r="E550" s="166"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9301,9 +9303,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="167"/>
+      <c r="D567" s="168"/>
+      <c r="E567" s="168"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9454,9 +9456,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="165"/>
+      <c r="D584" s="166"/>
+      <c r="E584" s="166"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9607,9 +9609,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="165"/>
+      <c r="D601" s="166"/>
+      <c r="E601" s="166"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -9760,9 +9762,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="165"/>
+      <c r="D618" s="166"/>
+      <c r="E618" s="166"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -9913,9 +9915,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="165"/>
+      <c r="D635" s="166"/>
+      <c r="E635" s="166"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10066,9 +10068,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="165"/>
+      <c r="D652" s="166"/>
+      <c r="E652" s="166"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10219,9 +10221,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="165"/>
+      <c r="D669" s="166"/>
+      <c r="E669" s="166"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10372,9 +10374,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="165"/>
+      <c r="D686" s="166"/>
+      <c r="E686" s="166"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10525,9 +10527,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="165"/>
+      <c r="D703" s="166"/>
+      <c r="E703" s="166"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -10678,9 +10680,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="165"/>
+      <c r="D720" s="166"/>
+      <c r="E720" s="166"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -10831,9 +10833,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="165"/>
+      <c r="D737" s="166"/>
+      <c r="E737" s="166"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -10984,9 +10986,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="165"/>
+      <c r="D754" s="166"/>
+      <c r="E754" s="166"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11137,9 +11139,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="165"/>
+      <c r="D771" s="166"/>
+      <c r="E771" s="166"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11290,9 +11292,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="165"/>
+      <c r="D788" s="166"/>
+      <c r="E788" s="166"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11443,9 +11445,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="165"/>
+      <c r="D805" s="166"/>
+      <c r="E805" s="166"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11596,18 +11598,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="177"/>
+      <c r="D822" s="178"/>
+      <c r="E822" s="178"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="165"/>
+      <c r="D823" s="166"/>
+      <c r="E823" s="166"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -11758,9 +11760,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="167"/>
+      <c r="D840" s="168"/>
+      <c r="E840" s="168"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -11911,9 +11913,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="165"/>
+      <c r="D857" s="166"/>
+      <c r="E857" s="166"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12064,9 +12066,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="165"/>
+      <c r="D874" s="166"/>
+      <c r="E874" s="166"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12217,9 +12219,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="165"/>
+      <c r="D891" s="166"/>
+      <c r="E891" s="166"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12370,9 +12372,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="165"/>
+      <c r="D908" s="166"/>
+      <c r="E908" s="166"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12523,9 +12525,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="165"/>
+      <c r="D925" s="166"/>
+      <c r="E925" s="166"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -12676,9 +12678,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="165"/>
+      <c r="D942" s="166"/>
+      <c r="E942" s="166"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -12829,9 +12831,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="165"/>
+      <c r="D959" s="166"/>
+      <c r="E959" s="166"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -12982,9 +12984,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="165"/>
+      <c r="D976" s="166"/>
+      <c r="E976" s="166"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13135,9 +13137,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="165"/>
+      <c r="D993" s="166"/>
+      <c r="E993" s="166"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13288,9 +13290,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="165"/>
+      <c r="D1010" s="166"/>
+      <c r="E1010" s="166"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13441,9 +13443,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="165"/>
+      <c r="D1027" s="166"/>
+      <c r="E1027" s="166"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13594,9 +13596,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="165"/>
+      <c r="D1044" s="166"/>
+      <c r="E1044" s="166"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -13747,9 +13749,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="165"/>
+      <c r="D1061" s="166"/>
+      <c r="E1061" s="166"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -13900,9 +13902,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="165"/>
+      <c r="D1078" s="166"/>
+      <c r="E1078" s="166"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14053,18 +14055,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="175"/>
+      <c r="D1095" s="176"/>
+      <c r="E1095" s="176"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="165"/>
+      <c r="D1096" s="166"/>
+      <c r="E1096" s="166"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14215,9 +14217,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="167"/>
+      <c r="D1113" s="168"/>
+      <c r="E1113" s="168"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14368,9 +14370,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="165"/>
+      <c r="D1130" s="166"/>
+      <c r="E1130" s="166"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14521,9 +14523,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="165"/>
+      <c r="D1147" s="166"/>
+      <c r="E1147" s="166"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -14674,9 +14676,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="165"/>
+      <c r="D1164" s="166"/>
+      <c r="E1164" s="166"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -14827,9 +14829,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="165"/>
+      <c r="D1181" s="166"/>
+      <c r="E1181" s="166"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -14980,9 +14982,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="165"/>
+      <c r="D1198" s="166"/>
+      <c r="E1198" s="166"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15133,9 +15135,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="165"/>
+      <c r="D1215" s="166"/>
+      <c r="E1215" s="166"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15286,9 +15288,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="165"/>
+      <c r="D1232" s="166"/>
+      <c r="E1232" s="166"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15439,9 +15441,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="165"/>
+      <c r="D1249" s="166"/>
+      <c r="E1249" s="166"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15592,9 +15594,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="165"/>
+      <c r="D1266" s="166"/>
+      <c r="E1266" s="166"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -15745,9 +15747,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="165"/>
+      <c r="D1283" s="166"/>
+      <c r="E1283" s="166"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -15898,9 +15900,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="165"/>
+      <c r="D1300" s="166"/>
+      <c r="E1300" s="166"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16051,9 +16053,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="165"/>
+      <c r="D1317" s="166"/>
+      <c r="E1317" s="166"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16204,9 +16206,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="165"/>
+      <c r="D1334" s="166"/>
+      <c r="E1334" s="166"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16357,9 +16359,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="165"/>
+      <c r="D1351" s="166"/>
+      <c r="E1351" s="166"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16510,18 +16512,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="173"/>
+      <c r="D1368" s="174"/>
+      <c r="E1368" s="174"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="165"/>
+      <c r="D1369" s="166"/>
+      <c r="E1369" s="166"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -16672,9 +16674,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="167"/>
+      <c r="D1386" s="168"/>
+      <c r="E1386" s="168"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -16825,9 +16827,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="165"/>
+      <c r="D1403" s="166"/>
+      <c r="E1403" s="166"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -16978,9 +16980,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="165"/>
+      <c r="D1420" s="166"/>
+      <c r="E1420" s="166"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17131,9 +17133,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="165"/>
+      <c r="D1437" s="166"/>
+      <c r="E1437" s="166"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17284,9 +17286,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="165"/>
+      <c r="D1454" s="166"/>
+      <c r="E1454" s="166"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17437,9 +17439,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="165"/>
+      <c r="D1471" s="166"/>
+      <c r="E1471" s="166"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17590,9 +17592,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="165"/>
+      <c r="D1488" s="166"/>
+      <c r="E1488" s="166"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -17743,9 +17745,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="165"/>
+      <c r="D1505" s="166"/>
+      <c r="E1505" s="166"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -17896,9 +17898,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="165"/>
+      <c r="D1522" s="166"/>
+      <c r="E1522" s="166"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18049,9 +18051,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="165"/>
+      <c r="D1539" s="166"/>
+      <c r="E1539" s="166"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18202,9 +18204,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="165"/>
+      <c r="D1556" s="166"/>
+      <c r="E1556" s="166"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18355,9 +18357,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="165"/>
+      <c r="D1573" s="166"/>
+      <c r="E1573" s="166"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18508,9 +18510,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="165"/>
+      <c r="D1590" s="166"/>
+      <c r="E1590" s="166"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -18661,9 +18663,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="165"/>
+      <c r="D1607" s="166"/>
+      <c r="E1607" s="166"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -18814,9 +18816,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="165"/>
+      <c r="D1624" s="166"/>
+      <c r="E1624" s="166"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -18967,18 +18969,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="170"/>
-      <c r="D1641" s="171"/>
-      <c r="E1641" s="171"/>
+      <c r="C1641" s="171"/>
+      <c r="D1641" s="172"/>
+      <c r="E1641" s="172"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="165"/>
+      <c r="D1642" s="166"/>
+      <c r="E1642" s="166"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19129,9 +19131,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="167"/>
+      <c r="D1659" s="168"/>
+      <c r="E1659" s="168"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19282,9 +19284,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="165"/>
+      <c r="D1676" s="166"/>
+      <c r="E1676" s="166"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19435,9 +19437,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="165"/>
+      <c r="D1693" s="166"/>
+      <c r="E1693" s="166"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19588,9 +19590,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="165"/>
+      <c r="D1710" s="166"/>
+      <c r="E1710" s="166"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -19741,9 +19743,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="165"/>
+      <c r="D1727" s="166"/>
+      <c r="E1727" s="166"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -19894,9 +19896,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="165"/>
+      <c r="D1744" s="166"/>
+      <c r="E1744" s="166"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20047,9 +20049,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="165"/>
+      <c r="D1761" s="166"/>
+      <c r="E1761" s="166"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20200,9 +20202,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="165"/>
+      <c r="D1778" s="166"/>
+      <c r="E1778" s="166"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20353,9 +20355,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="165"/>
+      <c r="D1795" s="166"/>
+      <c r="E1795" s="166"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20506,9 +20508,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="165"/>
+      <c r="D1812" s="166"/>
+      <c r="E1812" s="166"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -20659,9 +20661,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="165"/>
+      <c r="D1829" s="166"/>
+      <c r="E1829" s="166"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -20812,9 +20814,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="165"/>
+      <c r="D1846" s="166"/>
+      <c r="E1846" s="166"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -20965,9 +20967,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="165"/>
+      <c r="D1863" s="166"/>
+      <c r="E1863" s="166"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21118,9 +21120,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="165"/>
+      <c r="D1880" s="166"/>
+      <c r="E1880" s="166"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21271,9 +21273,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="165"/>
+      <c r="D1897" s="166"/>
+      <c r="E1897" s="166"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21424,18 +21426,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="168"/>
-      <c r="D1914" s="169"/>
-      <c r="E1914" s="169"/>
+      <c r="C1914" s="169"/>
+      <c r="D1914" s="170"/>
+      <c r="E1914" s="170"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="165"/>
+      <c r="D1915" s="166"/>
+      <c r="E1915" s="166"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21586,9 +21588,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="167"/>
+      <c r="D1932" s="168"/>
+      <c r="E1932" s="168"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -21739,9 +21741,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="165"/>
+      <c r="D1949" s="166"/>
+      <c r="E1949" s="166"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -21892,9 +21894,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="165"/>
+      <c r="D1966" s="166"/>
+      <c r="E1966" s="166"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22045,9 +22047,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="165"/>
+      <c r="D1983" s="166"/>
+      <c r="E1983" s="166"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22198,9 +22200,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="165"/>
+      <c r="D2000" s="166"/>
+      <c r="E2000" s="166"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22351,9 +22353,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="165"/>
+      <c r="D2017" s="166"/>
+      <c r="E2017" s="166"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22504,9 +22506,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="165"/>
+      <c r="D2034" s="166"/>
+      <c r="E2034" s="166"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22657,9 +22659,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="165"/>
+      <c r="D2051" s="166"/>
+      <c r="E2051" s="166"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -22810,9 +22812,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="165"/>
+      <c r="D2068" s="166"/>
+      <c r="E2068" s="166"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -22963,9 +22965,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="165"/>
+      <c r="D2085" s="166"/>
+      <c r="E2085" s="166"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23116,9 +23118,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="165"/>
+      <c r="D2102" s="166"/>
+      <c r="E2102" s="166"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23269,9 +23271,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="165"/>
+      <c r="D2119" s="166"/>
+      <c r="E2119" s="166"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23422,9 +23424,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="165"/>
+      <c r="D2136" s="166"/>
+      <c r="E2136" s="166"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23575,9 +23577,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="165"/>
+      <c r="D2153" s="166"/>
+      <c r="E2153" s="166"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -23728,9 +23730,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="165"/>
+      <c r="D2170" s="166"/>
+      <c r="E2170" s="166"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24041,51 +24043,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="192" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="189" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="189"/>
-      <c r="L2" s="190"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="190"/>
+      <c r="F2" s="190"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="190"/>
+      <c r="I2" s="190"/>
+      <c r="J2" s="190"/>
+      <c r="K2" s="190"/>
+      <c r="L2" s="191"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="186" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="187"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="188"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -24302,19 +24304,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="185" t="s">
+      <c r="A20" s="186" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="186"/>
-      <c r="C20" s="186"/>
-      <c r="D20" s="186"/>
-      <c r="E20" s="186"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="186"/>
-      <c r="H20" s="186"/>
-      <c r="I20" s="186"/>
-      <c r="J20" s="186"/>
-      <c r="K20" s="187"/>
+      <c r="B20" s="187"/>
+      <c r="C20" s="187"/>
+      <c r="D20" s="187"/>
+      <c r="E20" s="187"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="187"/>
+      <c r="I20" s="187"/>
+      <c r="J20" s="187"/>
+      <c r="K20" s="188"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -24531,19 +24533,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="185" t="s">
+      <c r="A37" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="186"/>
-      <c r="C37" s="186"/>
-      <c r="D37" s="186"/>
-      <c r="E37" s="186"/>
-      <c r="F37" s="186"/>
-      <c r="G37" s="186"/>
-      <c r="H37" s="186"/>
-      <c r="I37" s="186"/>
-      <c r="J37" s="186"/>
-      <c r="K37" s="187"/>
+      <c r="B37" s="187"/>
+      <c r="C37" s="187"/>
+      <c r="D37" s="187"/>
+      <c r="E37" s="187"/>
+      <c r="F37" s="187"/>
+      <c r="G37" s="187"/>
+      <c r="H37" s="187"/>
+      <c r="I37" s="187"/>
+      <c r="J37" s="187"/>
+      <c r="K37" s="188"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -24801,28 +24803,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="192"/>
+      <c r="A3" s="193"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="193"/>
+      <c r="A4" s="194"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="193"/>
+      <c r="A5" s="194"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="193"/>
+      <c r="A6" s="194"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="193"/>
+      <c r="A7" s="194"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="193"/>
+      <c r="A8" s="194"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="193"/>
+      <c r="A9" s="194"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="194"/>
+      <c r="A10" s="195"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25005,10 +25007,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="196" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="196"/>
+      <c r="C1" s="197"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25019,7 +25021,7 @@
       <c r="E2" s="117"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="198" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="129" t="s">
@@ -25033,7 +25035,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="198"/>
+      <c r="A4" s="199"/>
       <c r="B4" s="126" t="s">
         <v>159</v>
       </c>
@@ -25045,7 +25047,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="198"/>
+      <c r="A5" s="199"/>
       <c r="B5" s="126" t="s">
         <v>160</v>
       </c>
@@ -25054,7 +25056,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="198"/>
+      <c r="A6" s="199"/>
       <c r="B6" s="137" t="s">
         <v>201</v>
       </c>
@@ -25066,7 +25068,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="198"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="126" t="s">
         <v>169</v>
       </c>
@@ -25078,7 +25080,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="198"/>
+      <c r="A8" s="199"/>
       <c r="B8" s="126" t="s">
         <v>170</v>
       </c>
@@ -25087,7 +25089,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="199"/>
+      <c r="A9" s="200"/>
       <c r="B9" s="134" t="s">
         <v>161</v>
       </c>
@@ -25102,7 +25104,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="198" t="s">
         <v>200</v>
       </c>
       <c r="B11" s="129" t="s">
@@ -25116,7 +25118,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="198"/>
+      <c r="A12" s="199"/>
       <c r="B12" s="126" t="s">
         <v>159</v>
       </c>
@@ -25128,7 +25130,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="198"/>
+      <c r="A13" s="199"/>
       <c r="B13" s="126" t="s">
         <v>160</v>
       </c>
@@ -25137,7 +25139,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="198"/>
+      <c r="A14" s="199"/>
       <c r="B14" s="137" t="s">
         <v>201</v>
       </c>
@@ -25149,7 +25151,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="198"/>
+      <c r="A15" s="199"/>
       <c r="B15" s="126" t="s">
         <v>169</v>
       </c>
@@ -25161,7 +25163,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="198"/>
+      <c r="A16" s="199"/>
       <c r="B16" s="126" t="s">
         <v>170</v>
       </c>
@@ -25170,7 +25172,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="199"/>
+      <c r="A17" s="200"/>
       <c r="B17" s="134" t="s">
         <v>161</v>
       </c>
@@ -25185,7 +25187,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="198" t="s">
         <v>200</v>
       </c>
       <c r="B19" s="129" t="s">
@@ -25194,7 +25196,7 @@
       <c r="C19" s="128"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="198"/>
+      <c r="A20" s="199"/>
       <c r="B20" s="126" t="s">
         <v>159</v>
       </c>
@@ -25204,14 +25206,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="198"/>
+      <c r="A21" s="199"/>
       <c r="B21" s="126" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="198"/>
+      <c r="A22" s="199"/>
       <c r="B22" s="137" t="s">
         <v>201</v>
       </c>
@@ -25221,7 +25223,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="198"/>
+      <c r="A23" s="199"/>
       <c r="B23" s="126" t="s">
         <v>169</v>
       </c>
@@ -25231,14 +25233,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="198"/>
+      <c r="A24" s="199"/>
       <c r="B24" s="126" t="s">
         <v>170</v>
       </c>
       <c r="C24" s="130"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="199"/>
+      <c r="A25" s="200"/>
       <c r="B25" s="134" t="s">
         <v>161</v>
       </c>
@@ -25273,147 +25275,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="211"/>
       <c r="C1" s="116"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="207" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="207"/>
+      <c r="B2" s="208"/>
       <c r="C2" s="118"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="208" t="s">
+      <c r="A3" s="209" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="207"/>
+      <c r="B3" s="208"/>
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="213"/>
-      <c r="B4" s="214"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="215"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="211" t="s">
+      <c r="A5" s="212" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="212"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="218" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="218"/>
+      <c r="B7" s="219"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="216" t="s">
         <v>184</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="217"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="205" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="206"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204" t="s">
+      <c r="A12" s="205" t="s">
         <v>186</v>
       </c>
-      <c r="B12" s="205"/>
+      <c r="B12" s="206"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="205" t="s">
         <v>187</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="206"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="205" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="205"/>
+      <c r="B14" s="206"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="205" t="s">
         <v>189</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="206"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="204" t="s">
+      <c r="A16" s="205" t="s">
         <v>190</v>
       </c>
-      <c r="B16" s="205"/>
+      <c r="B16" s="206"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="200" t="s">
+      <c r="A17" s="201" t="s">
         <v>192</v>
       </c>
-      <c r="B17" s="201"/>
+      <c r="B17" s="202"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="218" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="218"/>
+      <c r="B19" s="219"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="216" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="217"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="204"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="204" t="s">
+      <c r="A23" s="205" t="s">
         <v>196</v>
       </c>
-      <c r="B23" s="205"/>
+      <c r="B23" s="206"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="205"/>
+      <c r="A24" s="205"/>
+      <c r="B24" s="206"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="205" t="s">
         <v>197</v>
       </c>
-      <c r="B25" s="205"/>
+      <c r="B25" s="206"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="204" t="s">
+      <c r="A26" s="205" t="s">
         <v>198</v>
       </c>
-      <c r="B26" s="205"/>
+      <c r="B26" s="206"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="200"/>
-      <c r="B27" s="201"/>
+      <c r="A27" s="201"/>
+      <c r="B27" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
SMB - 4-1 done
</commit_message>
<xml_diff>
--- a/trunk/SMB/SMB.xlsx
+++ b/trunk/SMB/SMB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="231">
   <si>
     <t>Notes</t>
   </si>
@@ -741,6 +741,18 @@
   <si>
     <t>Koopa Loads</t>
   </si>
+  <si>
+    <t>4-2 begin</t>
+  </si>
+  <si>
+    <t>87 = same</t>
+  </si>
+  <si>
+    <t>97 = late</t>
+  </si>
+  <si>
+    <t>94 = same</t>
+  </si>
 </sst>
 </file>
 
@@ -750,10 +762,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1672,34 +1691,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1707,202 +1726,202 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1912,10 +1931,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1936,152 +1955,155 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="37" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2392,8 +2414,8 @@
   <dimension ref="A1:K137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="6" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -2410,16 +2432,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="156" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="157"/>
+      <c r="C1" s="158" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="138"/>
       <c r="H1" s="139">
         <f>SUM(G1:G65520)</f>
@@ -2497,10 +2519,10 @@
       <c r="B5" s="145" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="155" t="s">
         <v>206</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="155"/>
       <c r="E5" s="145"/>
       <c r="F5" s="141"/>
       <c r="G5" s="138"/>
@@ -2516,12 +2538,12 @@
       <c r="B6" s="145" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="155" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="160"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="164"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
       <c r="G6" s="138"/>
       <c r="H6" s="138"/>
       <c r="I6" s="138"/>
@@ -2537,7 +2559,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="160" t="s">
         <v>204</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2557,7 +2579,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A9" s="156"/>
+      <c r="A9" s="161"/>
       <c r="B9" s="98" t="s">
         <v>175</v>
       </c>
@@ -2567,7 +2589,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A10" s="156"/>
+      <c r="A10" s="161"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2578,7 +2600,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A11" s="156"/>
+      <c r="A11" s="161"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2589,7 +2611,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A12" s="156"/>
+      <c r="A12" s="161"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2600,7 +2622,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A13" s="156"/>
+      <c r="A13" s="161"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2611,7 +2633,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A14" s="156"/>
+      <c r="A14" s="161"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2622,7 +2644,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1">
-      <c r="A15" s="156"/>
+      <c r="A15" s="161"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2633,7 +2655,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A16" s="156"/>
+      <c r="A16" s="161"/>
       <c r="B16" s="98" t="s">
         <v>177</v>
       </c>
@@ -2676,7 +2698,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="162" t="s">
         <v>209</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2696,7 +2718,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="156"/>
+      <c r="A20" s="161"/>
       <c r="B20" s="98" t="s">
         <v>175</v>
       </c>
@@ -2709,7 +2731,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A21" s="156"/>
+      <c r="A21" s="161"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2720,7 +2742,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A22" s="156"/>
+      <c r="A22" s="161"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2731,7 +2753,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A23" s="156"/>
+      <c r="A23" s="161"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2742,7 +2764,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A24" s="156"/>
+      <c r="A24" s="161"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2753,7 +2775,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A25" s="156"/>
+      <c r="A25" s="161"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2764,7 +2786,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A26" s="156"/>
+      <c r="A26" s="161"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2775,7 +2797,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A27" s="156"/>
+      <c r="A27" s="161"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2786,7 +2808,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A28" s="156"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2797,7 +2819,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A29" s="156"/>
+      <c r="A29" s="161"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2808,7 +2830,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A30" s="156"/>
+      <c r="A30" s="161"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2819,7 +2841,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A31" s="156"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2830,7 +2852,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A32" s="156"/>
+      <c r="A32" s="161"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2841,7 +2863,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A33" s="156"/>
+      <c r="A33" s="161"/>
       <c r="B33" s="98" t="s">
         <v>177</v>
       </c>
@@ -2880,7 +2902,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="164" t="s">
         <v>208</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2900,7 +2922,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A37" s="156"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="98" t="s">
         <v>175</v>
       </c>
@@ -2917,7 +2939,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A38" s="156"/>
+      <c r="A38" s="161"/>
       <c r="B38" s="153" t="s">
         <v>222</v>
       </c>
@@ -2934,7 +2956,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A39" s="156"/>
+      <c r="A39" s="161"/>
       <c r="B39" s="153" t="s">
         <v>223</v>
       </c>
@@ -2951,7 +2973,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A40" s="156"/>
+      <c r="A40" s="161"/>
       <c r="B40" s="154" t="s">
         <v>224</v>
       </c>
@@ -2966,7 +2988,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A41" s="156"/>
+      <c r="A41" s="161"/>
       <c r="B41" s="154" t="s">
         <v>226</v>
       </c>
@@ -2983,7 +3005,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A42" s="156"/>
+      <c r="A42" s="161"/>
       <c r="B42" s="154" t="s">
         <v>225</v>
       </c>
@@ -3000,7 +3022,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A43" s="156"/>
+      <c r="A43" s="161"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3011,7 +3033,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A44" s="156"/>
+      <c r="A44" s="161"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3022,7 +3044,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A45" s="156"/>
+      <c r="A45" s="161"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3033,7 +3055,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A46" s="156"/>
+      <c r="A46" s="161"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3044,7 +3066,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A47" s="156"/>
+      <c r="A47" s="161"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3055,7 +3077,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A48" s="156"/>
+      <c r="A48" s="161"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3065,8 +3087,8 @@
       </c>
       <c r="F48" s="105"/>
     </row>
-    <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="156"/>
+    <row r="49" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A49" s="161"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3076,8 +3098,8 @@
       </c>
       <c r="F49" s="105"/>
     </row>
-    <row r="50" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A50" s="156"/>
+    <row r="50" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A50" s="161"/>
       <c r="B50" s="100"/>
       <c r="C50" s="101"/>
       <c r="D50" s="101"/>
@@ -3087,8 +3109,8 @@
       </c>
       <c r="F50" s="105"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A51" s="156"/>
+    <row r="51" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A51" s="161"/>
       <c r="B51" s="98" t="s">
         <v>177</v>
       </c>
@@ -3100,7 +3122,7 @@
       </c>
       <c r="F51" s="104"/>
     </row>
-    <row r="52" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="52" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="A52" s="150" t="s">
         <v>211</v>
       </c>
@@ -3125,9 +3147,9 @@
         <v>-63</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="54" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A54" s="157" t="s">
+    <row r="53" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="54" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A54" s="162" t="s">
         <v>212</v>
       </c>
       <c r="B54" s="109" t="s">
@@ -3146,8 +3168,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A55" s="156"/>
+    <row r="55" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A55" s="161"/>
       <c r="B55" s="98" t="s">
         <v>175</v>
       </c>
@@ -3159,30 +3181,51 @@
       </c>
       <c r="F55" s="104"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A56" s="156"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
+    <row r="56" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
+      <c r="A56" s="161"/>
+      <c r="B56" s="220" t="s">
+        <v>224</v>
+      </c>
+      <c r="C56" s="101">
+        <v>26182</v>
+      </c>
+      <c r="D56" s="101">
+        <v>26309</v>
+      </c>
       <c r="E56" s="122">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="F56" s="105"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A57" s="156"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="101"/>
+      <c r="H56" t="s">
+        <v>228</v>
+      </c>
+      <c r="I56" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A57" s="161"/>
+      <c r="B57" s="220" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" s="101">
+        <v>26964</v>
+      </c>
+      <c r="D57" s="101">
+        <v>27090</v>
+      </c>
       <c r="E57" s="121">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="F57" s="105"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A58" s="156"/>
+      <c r="H57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A58" s="161"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3192,8 +3235,8 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A59" s="156"/>
+    <row r="59" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A59" s="161"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3203,8 +3246,8 @@
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A60" s="156"/>
+    <row r="60" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A60" s="161"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3214,8 +3257,8 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A61" s="156"/>
+    <row r="61" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A61" s="161"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3225,8 +3268,8 @@
       </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A62" s="156"/>
+    <row r="62" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A62" s="161"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3236,8 +3279,8 @@
       </c>
       <c r="F62" s="105"/>
     </row>
-    <row r="63" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A63" s="156"/>
+    <row r="63" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A63" s="161"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3247,8 +3290,8 @@
       </c>
       <c r="F63" s="105"/>
     </row>
-    <row r="64" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A64" s="156"/>
+    <row r="64" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A64" s="161"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3259,7 +3302,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A65" s="156"/>
+      <c r="A65" s="161"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3270,7 +3313,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A66" s="156"/>
+      <c r="A66" s="161"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3281,7 +3324,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A67" s="156"/>
+      <c r="A67" s="161"/>
       <c r="B67" s="100"/>
       <c r="C67" s="101"/>
       <c r="D67" s="101"/>
@@ -3292,7 +3335,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A68" s="156"/>
+      <c r="A68" s="161"/>
       <c r="B68" s="98" t="s">
         <v>177</v>
       </c>
@@ -3331,7 +3374,7 @@
     </row>
     <row r="70" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="71" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A71" s="155" t="s">
+      <c r="A71" s="164" t="s">
         <v>215</v>
       </c>
       <c r="B71" s="113" t="s">
@@ -3351,7 +3394,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A72" s="156"/>
+      <c r="A72" s="161"/>
       <c r="B72" s="98" t="s">
         <v>175</v>
       </c>
@@ -3364,7 +3407,7 @@
       <c r="F72" s="104"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A73" s="156"/>
+      <c r="A73" s="161"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3375,7 +3418,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A74" s="156"/>
+      <c r="A74" s="161"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3386,7 +3429,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A75" s="156"/>
+      <c r="A75" s="161"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3397,7 +3440,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A76" s="156"/>
+      <c r="A76" s="161"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3408,7 +3451,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A77" s="156"/>
+      <c r="A77" s="161"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3419,7 +3462,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A78" s="156"/>
+      <c r="A78" s="161"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3430,7 +3473,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A79" s="156"/>
+      <c r="A79" s="161"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3441,7 +3484,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A80" s="156"/>
+      <c r="A80" s="161"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3452,7 +3495,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A81" s="156"/>
+      <c r="A81" s="161"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3463,7 +3506,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A82" s="156"/>
+      <c r="A82" s="161"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3474,7 +3517,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A83" s="156"/>
+      <c r="A83" s="161"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3485,7 +3528,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A84" s="156"/>
+      <c r="A84" s="161"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3496,7 +3539,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A85" s="156"/>
+      <c r="A85" s="161"/>
       <c r="B85" s="98" t="s">
         <v>177</v>
       </c>
@@ -3535,7 +3578,7 @@
     </row>
     <row r="87" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="88" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A88" s="157" t="s">
+      <c r="A88" s="162" t="s">
         <v>214</v>
       </c>
       <c r="B88" s="109" t="s">
@@ -3555,7 +3598,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A89" s="156"/>
+      <c r="A89" s="161"/>
       <c r="B89" s="98" t="s">
         <v>175</v>
       </c>
@@ -3568,7 +3611,7 @@
       <c r="F89" s="104"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A90" s="156"/>
+      <c r="A90" s="161"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3579,7 +3622,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A91" s="156"/>
+      <c r="A91" s="161"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3590,7 +3633,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A92" s="156"/>
+      <c r="A92" s="161"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3601,7 +3644,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A93" s="156"/>
+      <c r="A93" s="161"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3612,7 +3655,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A94" s="156"/>
+      <c r="A94" s="161"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3623,7 +3666,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A95" s="156"/>
+      <c r="A95" s="161"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3634,7 +3677,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A96" s="156"/>
+      <c r="A96" s="161"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3645,7 +3688,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A97" s="156"/>
+      <c r="A97" s="161"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3656,7 +3699,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A98" s="156"/>
+      <c r="A98" s="161"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3667,7 +3710,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A99" s="156"/>
+      <c r="A99" s="161"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3678,7 +3721,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A100" s="156"/>
+      <c r="A100" s="161"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3689,7 +3732,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A101" s="156"/>
+      <c r="A101" s="161"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3700,7 +3743,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A102" s="156"/>
+      <c r="A102" s="161"/>
       <c r="B102" s="98" t="s">
         <v>177</v>
       </c>
@@ -3739,7 +3782,7 @@
     </row>
     <row r="104" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="105" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A105" s="155" t="s">
+      <c r="A105" s="164" t="s">
         <v>218</v>
       </c>
       <c r="B105" s="113" t="s">
@@ -3759,7 +3802,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A106" s="156"/>
+      <c r="A106" s="161"/>
       <c r="B106" s="98" t="s">
         <v>175</v>
       </c>
@@ -3772,7 +3815,7 @@
       <c r="F106" s="104"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A107" s="156"/>
+      <c r="A107" s="161"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3783,7 +3826,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A108" s="156"/>
+      <c r="A108" s="161"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3794,7 +3837,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A109" s="156"/>
+      <c r="A109" s="161"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3805,7 +3848,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A110" s="156"/>
+      <c r="A110" s="161"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3816,7 +3859,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A111" s="156"/>
+      <c r="A111" s="161"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3827,7 +3870,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A112" s="156"/>
+      <c r="A112" s="161"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3838,7 +3881,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A113" s="156"/>
+      <c r="A113" s="161"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3849,7 +3892,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A114" s="156"/>
+      <c r="A114" s="161"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3860,7 +3903,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A115" s="156"/>
+      <c r="A115" s="161"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3871,7 +3914,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A116" s="156"/>
+      <c r="A116" s="161"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3882,7 +3925,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A117" s="156"/>
+      <c r="A117" s="161"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -3893,7 +3936,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A118" s="156"/>
+      <c r="A118" s="161"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -3904,7 +3947,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A119" s="156"/>
+      <c r="A119" s="161"/>
       <c r="B119" s="98" t="s">
         <v>177</v>
       </c>
@@ -3943,7 +3986,7 @@
     </row>
     <row r="121" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="122" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A122" s="157" t="s">
+      <c r="A122" s="162" t="s">
         <v>220</v>
       </c>
       <c r="B122" s="109" t="s">
@@ -3963,7 +4006,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A123" s="156"/>
+      <c r="A123" s="161"/>
       <c r="B123" s="98" t="s">
         <v>175</v>
       </c>
@@ -3976,7 +4019,7 @@
       <c r="F123" s="104"/>
     </row>
     <row r="124" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A124" s="156"/>
+      <c r="A124" s="161"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -3987,7 +4030,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A125" s="156"/>
+      <c r="A125" s="161"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -3998,7 +4041,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A126" s="156"/>
+      <c r="A126" s="161"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4009,7 +4052,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A127" s="156"/>
+      <c r="A127" s="161"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4020,7 +4063,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A128" s="156"/>
+      <c r="A128" s="161"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4031,7 +4074,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A129" s="156"/>
+      <c r="A129" s="161"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4042,7 +4085,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A130" s="156"/>
+      <c r="A130" s="161"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4053,7 +4096,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A131" s="156"/>
+      <c r="A131" s="161"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4064,7 +4107,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A132" s="156"/>
+      <c r="A132" s="161"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4075,7 +4118,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A133" s="156"/>
+      <c r="A133" s="161"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4086,7 +4129,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A134" s="156"/>
+      <c r="A134" s="161"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4097,7 +4140,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A135" s="156"/>
+      <c r="A135" s="161"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4108,7 +4151,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A136" s="156"/>
+      <c r="A136" s="161"/>
       <c r="B136" s="98" t="s">
         <v>177</v>
       </c>
@@ -4147,18 +4190,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A105:A119"/>
+    <mergeCell ref="A71:A85"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A88:A102"/>
+    <mergeCell ref="A36:A51"/>
+    <mergeCell ref="A54:A68"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A105:A119"/>
-    <mergeCell ref="A71:A85"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A88:A102"/>
-    <mergeCell ref="A36:A51"/>
-    <mergeCell ref="A54:A68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4190,13 +4233,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4226,18 +4269,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="165"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4389,9 +4432,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="168"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="171"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4542,9 +4585,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="165"/>
-      <c r="D38" s="166"/>
-      <c r="E38" s="166"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -4695,9 +4738,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="165"/>
-      <c r="D55" s="166"/>
-      <c r="E55" s="166"/>
+      <c r="C55" s="168"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -4848,9 +4891,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="165"/>
-      <c r="D72" s="166"/>
-      <c r="E72" s="166"/>
+      <c r="C72" s="168"/>
+      <c r="D72" s="169"/>
+      <c r="E72" s="169"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5001,9 +5044,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="165"/>
-      <c r="D89" s="166"/>
-      <c r="E89" s="166"/>
+      <c r="C89" s="168"/>
+      <c r="D89" s="169"/>
+      <c r="E89" s="169"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5154,9 +5197,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="165"/>
-      <c r="D106" s="166"/>
-      <c r="E106" s="166"/>
+      <c r="C106" s="168"/>
+      <c r="D106" s="169"/>
+      <c r="E106" s="169"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5307,9 +5350,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="165"/>
-      <c r="D123" s="166"/>
-      <c r="E123" s="166"/>
+      <c r="C123" s="168"/>
+      <c r="D123" s="169"/>
+      <c r="E123" s="169"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5460,9 +5503,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="165"/>
-      <c r="D140" s="166"/>
-      <c r="E140" s="166"/>
+      <c r="C140" s="168"/>
+      <c r="D140" s="169"/>
+      <c r="E140" s="169"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5613,9 +5656,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="165"/>
-      <c r="D157" s="166"/>
-      <c r="E157" s="166"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="169"/>
+      <c r="E157" s="169"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -5766,9 +5809,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="165"/>
-      <c r="D174" s="166"/>
-      <c r="E174" s="166"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="169"/>
+      <c r="E174" s="169"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -5919,9 +5962,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="165"/>
-      <c r="D191" s="166"/>
-      <c r="E191" s="166"/>
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6072,9 +6115,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="165"/>
-      <c r="D208" s="166"/>
-      <c r="E208" s="166"/>
+      <c r="C208" s="168"/>
+      <c r="D208" s="169"/>
+      <c r="E208" s="169"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6225,9 +6268,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="165"/>
-      <c r="D225" s="166"/>
-      <c r="E225" s="166"/>
+      <c r="C225" s="168"/>
+      <c r="D225" s="169"/>
+      <c r="E225" s="169"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6378,9 +6421,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="165"/>
-      <c r="D242" s="166"/>
-      <c r="E242" s="166"/>
+      <c r="C242" s="168"/>
+      <c r="D242" s="169"/>
+      <c r="E242" s="169"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6531,9 +6574,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="165"/>
-      <c r="D259" s="166"/>
-      <c r="E259" s="166"/>
+      <c r="C259" s="168"/>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -6684,18 +6727,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="181"/>
-      <c r="D276" s="182"/>
-      <c r="E276" s="182"/>
+      <c r="C276" s="172"/>
+      <c r="D276" s="173"/>
+      <c r="E276" s="173"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="165"/>
-      <c r="D277" s="166"/>
-      <c r="E277" s="166"/>
+      <c r="C277" s="168"/>
+      <c r="D277" s="169"/>
+      <c r="E277" s="169"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -6846,9 +6889,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="167"/>
-      <c r="D294" s="168"/>
-      <c r="E294" s="168"/>
+      <c r="C294" s="170"/>
+      <c r="D294" s="171"/>
+      <c r="E294" s="171"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -6999,9 +7042,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="165"/>
-      <c r="D311" s="166"/>
-      <c r="E311" s="166"/>
+      <c r="C311" s="168"/>
+      <c r="D311" s="169"/>
+      <c r="E311" s="169"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7152,9 +7195,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="165"/>
-      <c r="D328" s="166"/>
-      <c r="E328" s="166"/>
+      <c r="C328" s="168"/>
+      <c r="D328" s="169"/>
+      <c r="E328" s="169"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7305,9 +7348,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="165"/>
-      <c r="D345" s="166"/>
-      <c r="E345" s="166"/>
+      <c r="C345" s="168"/>
+      <c r="D345" s="169"/>
+      <c r="E345" s="169"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7458,9 +7501,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="165"/>
-      <c r="D362" s="166"/>
-      <c r="E362" s="166"/>
+      <c r="C362" s="168"/>
+      <c r="D362" s="169"/>
+      <c r="E362" s="169"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7611,9 +7654,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="165"/>
-      <c r="D379" s="166"/>
-      <c r="E379" s="166"/>
+      <c r="C379" s="168"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -7764,9 +7807,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="165"/>
-      <c r="D396" s="166"/>
-      <c r="E396" s="166"/>
+      <c r="C396" s="168"/>
+      <c r="D396" s="169"/>
+      <c r="E396" s="169"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -7917,9 +7960,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="165"/>
-      <c r="D413" s="166"/>
-      <c r="E413" s="166"/>
+      <c r="C413" s="168"/>
+      <c r="D413" s="169"/>
+      <c r="E413" s="169"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8070,9 +8113,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="165"/>
-      <c r="D430" s="166"/>
-      <c r="E430" s="166"/>
+      <c r="C430" s="168"/>
+      <c r="D430" s="169"/>
+      <c r="E430" s="169"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8223,9 +8266,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="165"/>
-      <c r="D447" s="166"/>
-      <c r="E447" s="166"/>
+      <c r="C447" s="168"/>
+      <c r="D447" s="169"/>
+      <c r="E447" s="169"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8376,9 +8419,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="165"/>
-      <c r="D464" s="166"/>
-      <c r="E464" s="166"/>
+      <c r="C464" s="168"/>
+      <c r="D464" s="169"/>
+      <c r="E464" s="169"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8529,9 +8572,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="165"/>
-      <c r="D481" s="166"/>
-      <c r="E481" s="166"/>
+      <c r="C481" s="168"/>
+      <c r="D481" s="169"/>
+      <c r="E481" s="169"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -8682,9 +8725,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="165"/>
-      <c r="D498" s="166"/>
-      <c r="E498" s="166"/>
+      <c r="C498" s="168"/>
+      <c r="D498" s="169"/>
+      <c r="E498" s="169"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -8835,9 +8878,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="165"/>
-      <c r="D515" s="166"/>
-      <c r="E515" s="166"/>
+      <c r="C515" s="168"/>
+      <c r="D515" s="169"/>
+      <c r="E515" s="169"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -8988,9 +9031,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="165"/>
-      <c r="D532" s="166"/>
-      <c r="E532" s="166"/>
+      <c r="C532" s="168"/>
+      <c r="D532" s="169"/>
+      <c r="E532" s="169"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9141,18 +9184,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="179"/>
-      <c r="D549" s="180"/>
-      <c r="E549" s="180"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="165"/>
-      <c r="D550" s="166"/>
-      <c r="E550" s="166"/>
+      <c r="C550" s="168"/>
+      <c r="D550" s="169"/>
+      <c r="E550" s="169"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9303,9 +9346,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="167"/>
-      <c r="D567" s="168"/>
-      <c r="E567" s="168"/>
+      <c r="C567" s="170"/>
+      <c r="D567" s="171"/>
+      <c r="E567" s="171"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9456,9 +9499,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="165"/>
-      <c r="D584" s="166"/>
-      <c r="E584" s="166"/>
+      <c r="C584" s="168"/>
+      <c r="D584" s="169"/>
+      <c r="E584" s="169"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9609,9 +9652,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="165"/>
-      <c r="D601" s="166"/>
-      <c r="E601" s="166"/>
+      <c r="C601" s="168"/>
+      <c r="D601" s="169"/>
+      <c r="E601" s="169"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -9762,9 +9805,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="165"/>
-      <c r="D618" s="166"/>
-      <c r="E618" s="166"/>
+      <c r="C618" s="168"/>
+      <c r="D618" s="169"/>
+      <c r="E618" s="169"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -9915,9 +9958,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="165"/>
-      <c r="D635" s="166"/>
-      <c r="E635" s="166"/>
+      <c r="C635" s="168"/>
+      <c r="D635" s="169"/>
+      <c r="E635" s="169"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10068,9 +10111,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="165"/>
-      <c r="D652" s="166"/>
-      <c r="E652" s="166"/>
+      <c r="C652" s="168"/>
+      <c r="D652" s="169"/>
+      <c r="E652" s="169"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10221,9 +10264,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="165"/>
-      <c r="D669" s="166"/>
-      <c r="E669" s="166"/>
+      <c r="C669" s="168"/>
+      <c r="D669" s="169"/>
+      <c r="E669" s="169"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10374,9 +10417,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="165"/>
-      <c r="D686" s="166"/>
-      <c r="E686" s="166"/>
+      <c r="C686" s="168"/>
+      <c r="D686" s="169"/>
+      <c r="E686" s="169"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10527,9 +10570,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="165"/>
-      <c r="D703" s="166"/>
-      <c r="E703" s="166"/>
+      <c r="C703" s="168"/>
+      <c r="D703" s="169"/>
+      <c r="E703" s="169"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -10680,9 +10723,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="165"/>
-      <c r="D720" s="166"/>
-      <c r="E720" s="166"/>
+      <c r="C720" s="168"/>
+      <c r="D720" s="169"/>
+      <c r="E720" s="169"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -10833,9 +10876,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="165"/>
-      <c r="D737" s="166"/>
-      <c r="E737" s="166"/>
+      <c r="C737" s="168"/>
+      <c r="D737" s="169"/>
+      <c r="E737" s="169"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -10986,9 +11029,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="165"/>
-      <c r="D754" s="166"/>
-      <c r="E754" s="166"/>
+      <c r="C754" s="168"/>
+      <c r="D754" s="169"/>
+      <c r="E754" s="169"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11139,9 +11182,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="165"/>
-      <c r="D771" s="166"/>
-      <c r="E771" s="166"/>
+      <c r="C771" s="168"/>
+      <c r="D771" s="169"/>
+      <c r="E771" s="169"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11292,9 +11335,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="165"/>
-      <c r="D788" s="166"/>
-      <c r="E788" s="166"/>
+      <c r="C788" s="168"/>
+      <c r="D788" s="169"/>
+      <c r="E788" s="169"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11445,9 +11488,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="165"/>
-      <c r="D805" s="166"/>
-      <c r="E805" s="166"/>
+      <c r="C805" s="168"/>
+      <c r="D805" s="169"/>
+      <c r="E805" s="169"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11598,18 +11641,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="177"/>
-      <c r="D822" s="178"/>
-      <c r="E822" s="178"/>
+      <c r="C822" s="176"/>
+      <c r="D822" s="177"/>
+      <c r="E822" s="177"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="165"/>
-      <c r="D823" s="166"/>
-      <c r="E823" s="166"/>
+      <c r="C823" s="168"/>
+      <c r="D823" s="169"/>
+      <c r="E823" s="169"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -11760,9 +11803,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="167"/>
-      <c r="D840" s="168"/>
-      <c r="E840" s="168"/>
+      <c r="C840" s="170"/>
+      <c r="D840" s="171"/>
+      <c r="E840" s="171"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -11913,9 +11956,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="165"/>
-      <c r="D857" s="166"/>
-      <c r="E857" s="166"/>
+      <c r="C857" s="168"/>
+      <c r="D857" s="169"/>
+      <c r="E857" s="169"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12066,9 +12109,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="165"/>
-      <c r="D874" s="166"/>
-      <c r="E874" s="166"/>
+      <c r="C874" s="168"/>
+      <c r="D874" s="169"/>
+      <c r="E874" s="169"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12219,9 +12262,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="165"/>
-      <c r="D891" s="166"/>
-      <c r="E891" s="166"/>
+      <c r="C891" s="168"/>
+      <c r="D891" s="169"/>
+      <c r="E891" s="169"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12372,9 +12415,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="165"/>
-      <c r="D908" s="166"/>
-      <c r="E908" s="166"/>
+      <c r="C908" s="168"/>
+      <c r="D908" s="169"/>
+      <c r="E908" s="169"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12525,9 +12568,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="165"/>
-      <c r="D925" s="166"/>
-      <c r="E925" s="166"/>
+      <c r="C925" s="168"/>
+      <c r="D925" s="169"/>
+      <c r="E925" s="169"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -12678,9 +12721,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="165"/>
-      <c r="D942" s="166"/>
-      <c r="E942" s="166"/>
+      <c r="C942" s="168"/>
+      <c r="D942" s="169"/>
+      <c r="E942" s="169"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -12831,9 +12874,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="165"/>
-      <c r="D959" s="166"/>
-      <c r="E959" s="166"/>
+      <c r="C959" s="168"/>
+      <c r="D959" s="169"/>
+      <c r="E959" s="169"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -12984,9 +13027,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="165"/>
-      <c r="D976" s="166"/>
-      <c r="E976" s="166"/>
+      <c r="C976" s="168"/>
+      <c r="D976" s="169"/>
+      <c r="E976" s="169"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13137,9 +13180,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="165"/>
-      <c r="D993" s="166"/>
-      <c r="E993" s="166"/>
+      <c r="C993" s="168"/>
+      <c r="D993" s="169"/>
+      <c r="E993" s="169"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13290,9 +13333,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="165"/>
-      <c r="D1010" s="166"/>
-      <c r="E1010" s="166"/>
+      <c r="C1010" s="168"/>
+      <c r="D1010" s="169"/>
+      <c r="E1010" s="169"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13443,9 +13486,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="165"/>
-      <c r="D1027" s="166"/>
-      <c r="E1027" s="166"/>
+      <c r="C1027" s="168"/>
+      <c r="D1027" s="169"/>
+      <c r="E1027" s="169"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13596,9 +13639,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="165"/>
-      <c r="D1044" s="166"/>
-      <c r="E1044" s="166"/>
+      <c r="C1044" s="168"/>
+      <c r="D1044" s="169"/>
+      <c r="E1044" s="169"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -13749,9 +13792,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="165"/>
-      <c r="D1061" s="166"/>
-      <c r="E1061" s="166"/>
+      <c r="C1061" s="168"/>
+      <c r="D1061" s="169"/>
+      <c r="E1061" s="169"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -13902,9 +13945,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="165"/>
-      <c r="D1078" s="166"/>
-      <c r="E1078" s="166"/>
+      <c r="C1078" s="168"/>
+      <c r="D1078" s="169"/>
+      <c r="E1078" s="169"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14055,18 +14098,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="175"/>
-      <c r="D1095" s="176"/>
-      <c r="E1095" s="176"/>
+      <c r="C1095" s="178"/>
+      <c r="D1095" s="179"/>
+      <c r="E1095" s="179"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="165"/>
-      <c r="D1096" s="166"/>
-      <c r="E1096" s="166"/>
+      <c r="C1096" s="168"/>
+      <c r="D1096" s="169"/>
+      <c r="E1096" s="169"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14217,9 +14260,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="167"/>
-      <c r="D1113" s="168"/>
-      <c r="E1113" s="168"/>
+      <c r="C1113" s="170"/>
+      <c r="D1113" s="171"/>
+      <c r="E1113" s="171"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14370,9 +14413,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="165"/>
-      <c r="D1130" s="166"/>
-      <c r="E1130" s="166"/>
+      <c r="C1130" s="168"/>
+      <c r="D1130" s="169"/>
+      <c r="E1130" s="169"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14523,9 +14566,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="165"/>
-      <c r="D1147" s="166"/>
-      <c r="E1147" s="166"/>
+      <c r="C1147" s="168"/>
+      <c r="D1147" s="169"/>
+      <c r="E1147" s="169"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -14676,9 +14719,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="165"/>
-      <c r="D1164" s="166"/>
-      <c r="E1164" s="166"/>
+      <c r="C1164" s="168"/>
+      <c r="D1164" s="169"/>
+      <c r="E1164" s="169"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -14829,9 +14872,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="165"/>
-      <c r="D1181" s="166"/>
-      <c r="E1181" s="166"/>
+      <c r="C1181" s="168"/>
+      <c r="D1181" s="169"/>
+      <c r="E1181" s="169"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -14982,9 +15025,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="165"/>
-      <c r="D1198" s="166"/>
-      <c r="E1198" s="166"/>
+      <c r="C1198" s="168"/>
+      <c r="D1198" s="169"/>
+      <c r="E1198" s="169"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15135,9 +15178,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="165"/>
-      <c r="D1215" s="166"/>
-      <c r="E1215" s="166"/>
+      <c r="C1215" s="168"/>
+      <c r="D1215" s="169"/>
+      <c r="E1215" s="169"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15288,9 +15331,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="165"/>
-      <c r="D1232" s="166"/>
-      <c r="E1232" s="166"/>
+      <c r="C1232" s="168"/>
+      <c r="D1232" s="169"/>
+      <c r="E1232" s="169"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15441,9 +15484,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="165"/>
-      <c r="D1249" s="166"/>
-      <c r="E1249" s="166"/>
+      <c r="C1249" s="168"/>
+      <c r="D1249" s="169"/>
+      <c r="E1249" s="169"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15594,9 +15637,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="165"/>
-      <c r="D1266" s="166"/>
-      <c r="E1266" s="166"/>
+      <c r="C1266" s="168"/>
+      <c r="D1266" s="169"/>
+      <c r="E1266" s="169"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -15747,9 +15790,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="165"/>
-      <c r="D1283" s="166"/>
-      <c r="E1283" s="166"/>
+      <c r="C1283" s="168"/>
+      <c r="D1283" s="169"/>
+      <c r="E1283" s="169"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -15900,9 +15943,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="165"/>
-      <c r="D1300" s="166"/>
-      <c r="E1300" s="166"/>
+      <c r="C1300" s="168"/>
+      <c r="D1300" s="169"/>
+      <c r="E1300" s="169"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16053,9 +16096,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="165"/>
-      <c r="D1317" s="166"/>
-      <c r="E1317" s="166"/>
+      <c r="C1317" s="168"/>
+      <c r="D1317" s="169"/>
+      <c r="E1317" s="169"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16206,9 +16249,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="165"/>
-      <c r="D1334" s="166"/>
-      <c r="E1334" s="166"/>
+      <c r="C1334" s="168"/>
+      <c r="D1334" s="169"/>
+      <c r="E1334" s="169"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16359,9 +16402,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="165"/>
-      <c r="D1351" s="166"/>
-      <c r="E1351" s="166"/>
+      <c r="C1351" s="168"/>
+      <c r="D1351" s="169"/>
+      <c r="E1351" s="169"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16512,18 +16555,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="173"/>
-      <c r="D1368" s="174"/>
-      <c r="E1368" s="174"/>
+      <c r="C1368" s="180"/>
+      <c r="D1368" s="181"/>
+      <c r="E1368" s="181"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="165"/>
-      <c r="D1369" s="166"/>
-      <c r="E1369" s="166"/>
+      <c r="C1369" s="168"/>
+      <c r="D1369" s="169"/>
+      <c r="E1369" s="169"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -16674,9 +16717,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="167"/>
-      <c r="D1386" s="168"/>
-      <c r="E1386" s="168"/>
+      <c r="C1386" s="170"/>
+      <c r="D1386" s="171"/>
+      <c r="E1386" s="171"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -16827,9 +16870,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="165"/>
-      <c r="D1403" s="166"/>
-      <c r="E1403" s="166"/>
+      <c r="C1403" s="168"/>
+      <c r="D1403" s="169"/>
+      <c r="E1403" s="169"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -16980,9 +17023,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="165"/>
-      <c r="D1420" s="166"/>
-      <c r="E1420" s="166"/>
+      <c r="C1420" s="168"/>
+      <c r="D1420" s="169"/>
+      <c r="E1420" s="169"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17133,9 +17176,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="165"/>
-      <c r="D1437" s="166"/>
-      <c r="E1437" s="166"/>
+      <c r="C1437" s="168"/>
+      <c r="D1437" s="169"/>
+      <c r="E1437" s="169"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17286,9 +17329,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="165"/>
-      <c r="D1454" s="166"/>
-      <c r="E1454" s="166"/>
+      <c r="C1454" s="168"/>
+      <c r="D1454" s="169"/>
+      <c r="E1454" s="169"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17439,9 +17482,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="165"/>
-      <c r="D1471" s="166"/>
-      <c r="E1471" s="166"/>
+      <c r="C1471" s="168"/>
+      <c r="D1471" s="169"/>
+      <c r="E1471" s="169"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17592,9 +17635,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="165"/>
-      <c r="D1488" s="166"/>
-      <c r="E1488" s="166"/>
+      <c r="C1488" s="168"/>
+      <c r="D1488" s="169"/>
+      <c r="E1488" s="169"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -17745,9 +17788,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="165"/>
-      <c r="D1505" s="166"/>
-      <c r="E1505" s="166"/>
+      <c r="C1505" s="168"/>
+      <c r="D1505" s="169"/>
+      <c r="E1505" s="169"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -17898,9 +17941,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="165"/>
-      <c r="D1522" s="166"/>
-      <c r="E1522" s="166"/>
+      <c r="C1522" s="168"/>
+      <c r="D1522" s="169"/>
+      <c r="E1522" s="169"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18051,9 +18094,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="165"/>
-      <c r="D1539" s="166"/>
-      <c r="E1539" s="166"/>
+      <c r="C1539" s="168"/>
+      <c r="D1539" s="169"/>
+      <c r="E1539" s="169"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18204,9 +18247,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="165"/>
-      <c r="D1556" s="166"/>
-      <c r="E1556" s="166"/>
+      <c r="C1556" s="168"/>
+      <c r="D1556" s="169"/>
+      <c r="E1556" s="169"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18357,9 +18400,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="165"/>
-      <c r="D1573" s="166"/>
-      <c r="E1573" s="166"/>
+      <c r="C1573" s="168"/>
+      <c r="D1573" s="169"/>
+      <c r="E1573" s="169"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18510,9 +18553,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="165"/>
-      <c r="D1590" s="166"/>
-      <c r="E1590" s="166"/>
+      <c r="C1590" s="168"/>
+      <c r="D1590" s="169"/>
+      <c r="E1590" s="169"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -18663,9 +18706,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="165"/>
-      <c r="D1607" s="166"/>
-      <c r="E1607" s="166"/>
+      <c r="C1607" s="168"/>
+      <c r="D1607" s="169"/>
+      <c r="E1607" s="169"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -18816,9 +18859,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="165"/>
-      <c r="D1624" s="166"/>
-      <c r="E1624" s="166"/>
+      <c r="C1624" s="168"/>
+      <c r="D1624" s="169"/>
+      <c r="E1624" s="169"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -18969,18 +19012,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="171"/>
-      <c r="D1641" s="172"/>
-      <c r="E1641" s="172"/>
+      <c r="C1641" s="182"/>
+      <c r="D1641" s="183"/>
+      <c r="E1641" s="183"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="165"/>
-      <c r="D1642" s="166"/>
-      <c r="E1642" s="166"/>
+      <c r="C1642" s="168"/>
+      <c r="D1642" s="169"/>
+      <c r="E1642" s="169"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19131,9 +19174,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="167"/>
-      <c r="D1659" s="168"/>
-      <c r="E1659" s="168"/>
+      <c r="C1659" s="170"/>
+      <c r="D1659" s="171"/>
+      <c r="E1659" s="171"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19284,9 +19327,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="165"/>
-      <c r="D1676" s="166"/>
-      <c r="E1676" s="166"/>
+      <c r="C1676" s="168"/>
+      <c r="D1676" s="169"/>
+      <c r="E1676" s="169"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19437,9 +19480,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="165"/>
-      <c r="D1693" s="166"/>
-      <c r="E1693" s="166"/>
+      <c r="C1693" s="168"/>
+      <c r="D1693" s="169"/>
+      <c r="E1693" s="169"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19590,9 +19633,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="165"/>
-      <c r="D1710" s="166"/>
-      <c r="E1710" s="166"/>
+      <c r="C1710" s="168"/>
+      <c r="D1710" s="169"/>
+      <c r="E1710" s="169"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -19743,9 +19786,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="165"/>
-      <c r="D1727" s="166"/>
-      <c r="E1727" s="166"/>
+      <c r="C1727" s="168"/>
+      <c r="D1727" s="169"/>
+      <c r="E1727" s="169"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -19896,9 +19939,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="165"/>
-      <c r="D1744" s="166"/>
-      <c r="E1744" s="166"/>
+      <c r="C1744" s="168"/>
+      <c r="D1744" s="169"/>
+      <c r="E1744" s="169"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20049,9 +20092,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="165"/>
-      <c r="D1761" s="166"/>
-      <c r="E1761" s="166"/>
+      <c r="C1761" s="168"/>
+      <c r="D1761" s="169"/>
+      <c r="E1761" s="169"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20202,9 +20245,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="165"/>
-      <c r="D1778" s="166"/>
-      <c r="E1778" s="166"/>
+      <c r="C1778" s="168"/>
+      <c r="D1778" s="169"/>
+      <c r="E1778" s="169"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20355,9 +20398,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="165"/>
-      <c r="D1795" s="166"/>
-      <c r="E1795" s="166"/>
+      <c r="C1795" s="168"/>
+      <c r="D1795" s="169"/>
+      <c r="E1795" s="169"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20508,9 +20551,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="165"/>
-      <c r="D1812" s="166"/>
-      <c r="E1812" s="166"/>
+      <c r="C1812" s="168"/>
+      <c r="D1812" s="169"/>
+      <c r="E1812" s="169"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -20661,9 +20704,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="165"/>
-      <c r="D1829" s="166"/>
-      <c r="E1829" s="166"/>
+      <c r="C1829" s="168"/>
+      <c r="D1829" s="169"/>
+      <c r="E1829" s="169"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -20814,9 +20857,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="165"/>
-      <c r="D1846" s="166"/>
-      <c r="E1846" s="166"/>
+      <c r="C1846" s="168"/>
+      <c r="D1846" s="169"/>
+      <c r="E1846" s="169"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -20967,9 +21010,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="165"/>
-      <c r="D1863" s="166"/>
-      <c r="E1863" s="166"/>
+      <c r="C1863" s="168"/>
+      <c r="D1863" s="169"/>
+      <c r="E1863" s="169"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21120,9 +21163,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="165"/>
-      <c r="D1880" s="166"/>
-      <c r="E1880" s="166"/>
+      <c r="C1880" s="168"/>
+      <c r="D1880" s="169"/>
+      <c r="E1880" s="169"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21273,9 +21316,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="165"/>
-      <c r="D1897" s="166"/>
-      <c r="E1897" s="166"/>
+      <c r="C1897" s="168"/>
+      <c r="D1897" s="169"/>
+      <c r="E1897" s="169"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21426,18 +21469,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="169"/>
-      <c r="D1914" s="170"/>
-      <c r="E1914" s="170"/>
+      <c r="C1914" s="184"/>
+      <c r="D1914" s="185"/>
+      <c r="E1914" s="185"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="165"/>
-      <c r="D1915" s="166"/>
-      <c r="E1915" s="166"/>
+      <c r="C1915" s="168"/>
+      <c r="D1915" s="169"/>
+      <c r="E1915" s="169"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21588,9 +21631,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="167"/>
-      <c r="D1932" s="168"/>
-      <c r="E1932" s="168"/>
+      <c r="C1932" s="170"/>
+      <c r="D1932" s="171"/>
+      <c r="E1932" s="171"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -21741,9 +21784,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="165"/>
-      <c r="D1949" s="166"/>
-      <c r="E1949" s="166"/>
+      <c r="C1949" s="168"/>
+      <c r="D1949" s="169"/>
+      <c r="E1949" s="169"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -21894,9 +21937,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="165"/>
-      <c r="D1966" s="166"/>
-      <c r="E1966" s="166"/>
+      <c r="C1966" s="168"/>
+      <c r="D1966" s="169"/>
+      <c r="E1966" s="169"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22047,9 +22090,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="165"/>
-      <c r="D1983" s="166"/>
-      <c r="E1983" s="166"/>
+      <c r="C1983" s="168"/>
+      <c r="D1983" s="169"/>
+      <c r="E1983" s="169"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22200,9 +22243,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="165"/>
-      <c r="D2000" s="166"/>
-      <c r="E2000" s="166"/>
+      <c r="C2000" s="168"/>
+      <c r="D2000" s="169"/>
+      <c r="E2000" s="169"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22353,9 +22396,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="165"/>
-      <c r="D2017" s="166"/>
-      <c r="E2017" s="166"/>
+      <c r="C2017" s="168"/>
+      <c r="D2017" s="169"/>
+      <c r="E2017" s="169"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22506,9 +22549,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="165"/>
-      <c r="D2034" s="166"/>
-      <c r="E2034" s="166"/>
+      <c r="C2034" s="168"/>
+      <c r="D2034" s="169"/>
+      <c r="E2034" s="169"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22659,9 +22702,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="165"/>
-      <c r="D2051" s="166"/>
-      <c r="E2051" s="166"/>
+      <c r="C2051" s="168"/>
+      <c r="D2051" s="169"/>
+      <c r="E2051" s="169"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -22812,9 +22855,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="165"/>
-      <c r="D2068" s="166"/>
-      <c r="E2068" s="166"/>
+      <c r="C2068" s="168"/>
+      <c r="D2068" s="169"/>
+      <c r="E2068" s="169"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -22965,9 +23008,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="165"/>
-      <c r="D2085" s="166"/>
-      <c r="E2085" s="166"/>
+      <c r="C2085" s="168"/>
+      <c r="D2085" s="169"/>
+      <c r="E2085" s="169"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23118,9 +23161,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="165"/>
-      <c r="D2102" s="166"/>
-      <c r="E2102" s="166"/>
+      <c r="C2102" s="168"/>
+      <c r="D2102" s="169"/>
+      <c r="E2102" s="169"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23271,9 +23314,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="165"/>
-      <c r="D2119" s="166"/>
-      <c r="E2119" s="166"/>
+      <c r="C2119" s="168"/>
+      <c r="D2119" s="169"/>
+      <c r="E2119" s="169"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23424,9 +23467,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="165"/>
-      <c r="D2136" s="166"/>
-      <c r="E2136" s="166"/>
+      <c r="C2136" s="168"/>
+      <c r="D2136" s="169"/>
+      <c r="E2136" s="169"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23577,9 +23620,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="165"/>
-      <c r="D2153" s="166"/>
-      <c r="E2153" s="166"/>
+      <c r="C2153" s="168"/>
+      <c r="D2153" s="169"/>
+      <c r="E2153" s="169"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -23730,9 +23773,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="165"/>
-      <c r="D2170" s="166"/>
-      <c r="E2170" s="166"/>
+      <c r="C2170" s="168"/>
+      <c r="D2170" s="169"/>
+      <c r="E2170" s="169"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -23880,26 +23923,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -23912,113 +24040,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24769,7 +24812,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24980,7 +25023,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25253,7 +25296,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25275,163 +25318,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="211" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="211"/>
+      <c r="B1" s="212"/>
       <c r="C1" s="116"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="217" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="208"/>
+      <c r="B2" s="218"/>
       <c r="C2" s="118"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="219" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="208"/>
+      <c r="B3" s="218"/>
       <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="214"/>
-      <c r="B4" s="215"/>
+      <c r="A4" s="215"/>
+      <c r="B4" s="216"/>
       <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="212" t="s">
+      <c r="A5" s="213" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="213"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="118"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="218" t="s">
+      <c r="A7" s="205" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="219"/>
+      <c r="B7" s="206"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="118"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="216" t="s">
+      <c r="A9" s="207" t="s">
         <v>184</v>
       </c>
-      <c r="B9" s="217"/>
+      <c r="B9" s="208"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="209"/>
+      <c r="B10" s="210"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="201" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="206"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="205" t="s">
+      <c r="A12" s="201" t="s">
         <v>186</v>
       </c>
-      <c r="B12" s="206"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="201" t="s">
         <v>187</v>
       </c>
-      <c r="B13" s="206"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="205" t="s">
+      <c r="A14" s="201" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="206"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="205" t="s">
+      <c r="A15" s="201" t="s">
         <v>189</v>
       </c>
-      <c r="B15" s="206"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="205" t="s">
+      <c r="A16" s="201" t="s">
         <v>190</v>
       </c>
-      <c r="B16" s="206"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="201" t="s">
+      <c r="A17" s="203" t="s">
         <v>192</v>
       </c>
-      <c r="B17" s="202"/>
+      <c r="B17" s="204"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="218" t="s">
+      <c r="A19" s="205" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="219"/>
+      <c r="B19" s="206"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="118"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="216" t="s">
+      <c r="A21" s="207" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="217"/>
+      <c r="B21" s="208"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="210"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="205" t="s">
+      <c r="A23" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B23" s="206"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="205"/>
-      <c r="B24" s="206"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="205" t="s">
+      <c r="A25" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B25" s="206"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="205" t="s">
+      <c r="A26" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B26" s="206"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="201"/>
-      <c r="B27" s="202"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25442,6 +25472,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>